<commit_message>
solucionado lo de las fechas y lo de los datos ambulantes del excel aparte que se añadio el formato a las celdas
</commit_message>
<xml_diff>
--- a/packages/api/public/plantilla-archivos.xlsx
+++ b/packages/api/public/plantilla-archivos.xlsx
@@ -37,16 +37,17 @@
     <t xml:space="preserve">FECHA DE RECIBO</t>
   </si>
   <si>
-    <t xml:space="preserve">PATOLOGIA*</t>
+    <t xml:space="preserve">PATOLOGIA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -126,12 +127,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -140,6 +145,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -163,36 +172,36 @@
   <dimension ref="B2:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.09"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>